<commit_message>
At this point it gives us all the tabs, all the columns in order, with CollectionDevice and CalibrationDate missing
</commit_message>
<xml_diff>
--- a/input/RelationshipMap.xlsx
+++ b/input/RelationshipMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toled\Desktop\SCCWRP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itlender/Projects/BLM_data_reformatter/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C599F1-8B05-4E95-ABD3-5F4944ED6019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E801EC3E-E88E-9B42-88EF-6468AA70A949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57300" yWindow="885" windowWidth="23160" windowHeight="11910" activeTab="1" xr2:uid="{F9812EE0-3961-FE4F-824E-79A3DFBA05C9}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{F9812EE0-3961-FE4F-824E-79A3DFBA05C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Analytes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="191">
   <si>
     <t>Temperature</t>
   </si>
@@ -294,15 +294,6 @@
     <t>HabitatReplicate</t>
   </si>
   <si>
-    <t>HabitatCollectionDepth</t>
-  </si>
-  <si>
-    <t>HabitatUnitCollectionDepth</t>
-  </si>
-  <si>
-    <t>HabitatPositionWaterColumn</t>
-  </si>
-  <si>
     <t>HabitatMethodName</t>
   </si>
   <si>
@@ -360,9 +351,6 @@
     <t>GPSFix</t>
   </si>
   <si>
-    <t>NR</t>
-  </si>
-  <si>
     <t>NR is just the default value. We don’t have that column I don’t think.</t>
   </si>
   <si>
@@ -465,27 +453,6 @@
     <t>FlowmeterSect1DepthUnit</t>
   </si>
   <si>
-    <t>FlowMeterSect2DepthUnit</t>
-  </si>
-  <si>
-    <t>FlowMeterSect3DepthUnit</t>
-  </si>
-  <si>
-    <t>FlowMeterSect4DepthUnit</t>
-  </si>
-  <si>
-    <t>FlowMeterSect1VelocityUnit</t>
-  </si>
-  <si>
-    <t>FlowMeterSect2VelocityUnit</t>
-  </si>
-  <si>
-    <t>FlowMeterSect3VelocityUnit</t>
-  </si>
-  <si>
-    <t>FlowMeterSect4VelocityUnit</t>
-  </si>
-  <si>
     <t>FieldResults, HabitatResults</t>
   </si>
   <si>
@@ -604,6 +571,42 @@
   </si>
   <si>
     <t>FieldResult</t>
+  </si>
+  <si>
+    <t>FlowmeterSect2DepthUnit</t>
+  </si>
+  <si>
+    <t>FlowmeterSect3DepthUnit</t>
+  </si>
+  <si>
+    <t>FlowmeterSect4DepthUnit</t>
+  </si>
+  <si>
+    <t>FlowmeterSect1VelocityUnit</t>
+  </si>
+  <si>
+    <t>FlowmeterSect2VelocityUnit</t>
+  </si>
+  <si>
+    <t>FlowmeterSect3VelocityUnit</t>
+  </si>
+  <si>
+    <t>FlowmeterSect4VelocityUnit</t>
+  </si>
+  <si>
+    <t>FieldCollectionComments</t>
+  </si>
+  <si>
+    <t>InstrumentCalibrationDate</t>
+  </si>
+  <si>
+    <t>CalibrationDate</t>
+  </si>
+  <si>
+    <t>HabitatCollectionComments</t>
+  </si>
+  <si>
+    <t>WithIn10SecondsOfMap</t>
   </si>
 </sst>
 </file>
@@ -997,22 +1000,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71EBA9C-90F2-5945-896F-0A96C8D71702}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.625" customWidth="1"/>
-    <col min="4" max="4" width="27.625" customWidth="1"/>
-    <col min="5" max="5" width="59.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="59.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>30</v>
@@ -1035,7 +1038,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
@@ -1058,9 +1061,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1069,7 +1072,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -1078,10 +1081,10 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
         <v>30</v>
@@ -1104,7 +1107,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
@@ -1124,12 +1127,12 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1138,7 +1141,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
@@ -1147,10 +1150,10 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
@@ -1173,7 +1176,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -1196,9 +1199,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1207,7 +1210,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E9" t="s">
         <v>30</v>
@@ -1216,10 +1219,10 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
         <v>30</v>
@@ -1242,9 +1245,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -1253,7 +1256,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -1262,12 +1265,12 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1276,7 +1279,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E12" t="s">
         <v>30</v>
@@ -1288,9 +1291,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -1299,7 +1302,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
@@ -1308,7 +1311,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1319,7 +1322,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
@@ -1331,9 +1334,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -1342,7 +1345,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
         <v>30</v>
@@ -1351,10 +1354,10 @@
         <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
@@ -1377,7 +1380,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1388,7 +1391,7 @@
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
         <v>32</v>
@@ -1400,9 +1403,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
@@ -1411,7 +1414,7 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E18" t="s">
         <v>35</v>
@@ -1423,9 +1426,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
@@ -1434,7 +1437,7 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>179</v>
       </c>
       <c r="E19" t="s">
         <v>36</v>
@@ -1446,9 +1449,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
@@ -1457,7 +1460,7 @@
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="E20" t="s">
         <v>37</v>
@@ -1469,9 +1472,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
@@ -1480,7 +1483,7 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="E21" t="s">
         <v>38</v>
@@ -1492,9 +1495,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
@@ -1503,7 +1506,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="E22" t="s">
         <v>35</v>
@@ -1515,9 +1518,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B23" t="s">
         <v>39</v>
@@ -1526,7 +1529,7 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="E23" t="s">
         <v>36</v>
@@ -1538,9 +1541,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>
@@ -1549,7 +1552,7 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="E24" t="s">
         <v>37</v>
@@ -1561,9 +1564,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B25" t="s">
         <v>39</v>
@@ -1572,7 +1575,7 @@
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="E25" t="s">
         <v>38</v>
@@ -1584,7 +1587,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1595,7 +1598,7 @@
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E26" t="s">
         <v>30</v>
@@ -1607,7 +1610,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1618,7 +1621,7 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E27" t="s">
         <v>30</v>
@@ -1630,7 +1633,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E28" t="s">
         <v>30</v>
@@ -1653,7 +1656,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1664,7 +1667,7 @@
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E29" t="s">
         <v>30</v>
@@ -1676,7 +1679,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E30" t="s">
         <v>30</v>
@@ -1699,7 +1702,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E31" t="s">
         <v>30</v>
@@ -1722,7 +1725,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E32" t="s">
         <v>30</v>
@@ -1745,7 +1748,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1756,7 +1759,7 @@
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E33" t="s">
         <v>30</v>
@@ -1768,9 +1771,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
         <v>50</v>
@@ -1779,7 +1782,7 @@
         <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E34" t="s">
         <v>30</v>
@@ -1791,7 +1794,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -1802,7 +1805,7 @@
         <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E35" t="s">
         <v>30</v>
@@ -1814,7 +1817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -1825,7 +1828,7 @@
         <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E36" t="s">
         <v>30</v>
@@ -1837,7 +1840,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>29</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E37" t="s">
         <v>30</v>
@@ -1860,7 +1863,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E38" t="s">
         <v>30</v>
@@ -1891,25 +1894,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227F44FB-EC10-E34D-B181-672CA1B29D12}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="134.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="134.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>19</v>
@@ -1926,7 +1929,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1934,10 +1937,10 @@
         <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1945,10 +1948,10 @@
         <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1956,10 +1959,10 @@
         <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1967,10 +1970,10 @@
         <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -1978,10 +1981,10 @@
         <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1989,10 +1992,10 @@
         <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -2000,10 +2003,10 @@
         <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2011,10 +2014,10 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -2022,10 +2025,10 @@
         <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -2047,24 +2050,24 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B13" t="s">
         <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -2075,7 +2078,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -2086,7 +2089,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -2108,285 +2111,285 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>71</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>68</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
       </c>
       <c r="D21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>186</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>189</v>
       </c>
       <c r="D25" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B29" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
       </c>
       <c r="D30" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>150</v>
-      </c>
-      <c r="E30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A31" t="s">
-        <v>154</v>
-      </c>
-      <c r="C31" t="s">
-        <v>133</v>
-      </c>
-      <c r="D31" t="s">
-        <v>150</v>
-      </c>
-      <c r="E31" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A32" t="s">
-        <v>155</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" t="s">
-        <v>150</v>
-      </c>
-      <c r="E32" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A33" t="s">
-        <v>161</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E33" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>90</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>90</v>
       </c>
-      <c r="D35" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A36" t="s">
+      <c r="D38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>91</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>91</v>
       </c>
-      <c r="D36" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A37" t="s">
+      <c r="D39" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>92</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>92</v>
       </c>
-      <c r="D37" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A38" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D39" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40" t="s">
-        <v>95</v>
-      </c>
       <c r="D40" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -2394,304 +2397,315 @@
         <v>31</v>
       </c>
       <c r="D41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" t="s">
+        <v>110</v>
+      </c>
+      <c r="E50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" t="s">
+        <v>110</v>
+      </c>
+      <c r="E51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A42" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" t="s">
-        <v>96</v>
-      </c>
-      <c r="D42" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A43" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A44" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" t="s">
-        <v>98</v>
-      </c>
-      <c r="D44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A45" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" t="s">
-        <v>100</v>
-      </c>
-      <c r="D46" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A47" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A48" t="s">
-        <v>105</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="D55" t="s">
         <v>110</v>
       </c>
-      <c r="D48" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A49" t="s">
-        <v>106</v>
-      </c>
-      <c r="B49" t="s">
-        <v>111</v>
-      </c>
-      <c r="D49" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A50" t="s">
-        <v>107</v>
-      </c>
-      <c r="C50" t="s">
-        <v>108</v>
-      </c>
-      <c r="D50" t="s">
-        <v>114</v>
-      </c>
-      <c r="E50" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A51" t="s">
-        <v>102</v>
-      </c>
-      <c r="B51" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51" t="s">
-        <v>114</v>
-      </c>
-      <c r="E51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A52" t="s">
-        <v>112</v>
-      </c>
-      <c r="B52" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A53" t="s">
+      <c r="E55" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>113</v>
       </c>
-      <c r="B53" t="s">
-        <v>113</v>
-      </c>
-      <c r="D53" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A54" t="s">
+      <c r="B56" t="s">
         <v>115</v>
       </c>
-      <c r="B54" t="s">
-        <v>115</v>
-      </c>
-      <c r="D54" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A55" t="s">
+      <c r="D56" t="s">
+        <v>110</v>
+      </c>
+      <c r="E56" t="s">
         <v>116</v>
       </c>
-      <c r="B55" t="s">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>118</v>
       </c>
-      <c r="D55" t="s">
-        <v>114</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="B58" t="s">
+        <v>118</v>
+      </c>
+      <c r="D58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A56" t="s">
-        <v>117</v>
-      </c>
-      <c r="B56" t="s">
-        <v>119</v>
-      </c>
-      <c r="D56" t="s">
-        <v>114</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="B60" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A57" t="s">
+      <c r="D60" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>121</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B61" t="s">
         <v>121</v>
       </c>
-      <c r="D57" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A58" t="s">
+      <c r="D61" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>122</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B63" t="s">
         <v>122</v>
       </c>
-      <c r="D58" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A59" t="s">
+      <c r="D63" t="s">
         <v>123</v>
       </c>
-      <c r="B59" t="s">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" t="s">
         <v>123</v>
       </c>
-      <c r="D59" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A60" t="s">
-        <v>124</v>
-      </c>
-      <c r="B60" t="s">
-        <v>124</v>
-      </c>
-      <c r="D60" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A61" t="s">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>125</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B65" t="s">
         <v>125</v>
       </c>
-      <c r="D61" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A62" t="s">
-        <v>126</v>
-      </c>
-      <c r="B62" t="s">
-        <v>126</v>
-      </c>
-      <c r="D62" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A63" t="s">
-        <v>128</v>
-      </c>
-      <c r="B63" t="s">
-        <v>128</v>
-      </c>
-      <c r="D63" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A64" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" t="s">
-        <v>129</v>
-      </c>
-      <c r="D64" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A65" t="s">
-        <v>165</v>
-      </c>
-      <c r="B65" t="s">
-        <v>167</v>
-      </c>
       <c r="D65" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B66" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D66" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>155</v>
+      </c>
+      <c r="B67" t="s">
+        <v>156</v>
+      </c>
+      <c r="D67" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>22</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>23</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>